<commit_message>
VRU economics MSCFD Fix
</commit_message>
<xml_diff>
--- a/downloads/notebooks/sample_data/VRU_Declining_Economics-Sim_Results.xlsx
+++ b/downloads/notebooks/sample_data/VRU_Declining_Economics-Sim_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricKim\Documents\aegis4048.github.io-source\content\downloads\notebooks\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B5C359-71FB-4A1E-8C14-DB031634D7C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF28659-087E-494E-BEFA-2CC79CE22E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="7" xr2:uid="{019FB55A-2F6E-496A-863D-C276009415F0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{019FB55A-2F6E-496A-863D-C276009415F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Gas Economics Calcualtor -  HT" sheetId="14" r:id="rId1"/>
@@ -270,9 +270,6 @@
     </r>
   </si>
   <si>
-    <t>Monthly Vol. [MCFD]</t>
-  </si>
-  <si>
     <t>Btu/SCF</t>
   </si>
   <si>
@@ -292,9 +289,6 @@
   </si>
   <si>
     <t>VRU Rental [$]</t>
-  </si>
-  <si>
-    <t>Daily Vol. [MCFD]</t>
   </si>
   <si>
     <t>Gross Rev. [$]</t>
@@ -487,6 +481,12 @@
   </si>
   <si>
     <t>[$/MMBtu]</t>
+  </si>
+  <si>
+    <t>Monthly Vol. [MSCF]</t>
+  </si>
+  <si>
+    <t>Daily Vol. [MSCFD]</t>
   </si>
 </sst>
 </file>
@@ -1820,7 +1820,7 @@
   <dimension ref="B2:AD66"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,7 +1841,7 @@
   <sheetData>
     <row r="2" spans="2:30" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="140" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" s="140"/>
       <c r="D2" s="140"/>
@@ -1856,37 +1856,37 @@
     </row>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="76" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="76" t="s">
+      <c r="F3" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="G3" s="76" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="76" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="76" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="76" t="s">
+      <c r="I3" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="76" t="s">
+      <c r="J3" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="76" t="s">
+      <c r="K3" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="J3" s="76" t="s">
+      <c r="L3" s="76" t="s">
         <v>64</v>
-      </c>
-      <c r="K3" s="76" t="s">
-        <v>65</v>
-      </c>
-      <c r="L3" s="76" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.25">
@@ -1894,34 +1894,34 @@
         <v>32</v>
       </c>
       <c r="C4" s="80" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="D4" s="80" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="80" t="s">
+      <c r="F4" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="80" t="s">
+      <c r="H4" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="80" t="s">
+      <c r="I4" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="80" t="s">
+      <c r="J4" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="80" t="s">
         <v>51</v>
-      </c>
-      <c r="J4" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" s="81" t="s">
-        <v>55</v>
-      </c>
-      <c r="L4" s="80" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
@@ -18158,8 +18158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E0FC7EE-5E46-4B2E-B243-83A2082E9CE0}">
   <dimension ref="B1:AD65"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18180,7 +18180,7 @@
   <sheetData>
     <row r="1" spans="2:30" ht="45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="140" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C1" s="140"/>
       <c r="D1" s="140"/>
@@ -18195,37 +18195,37 @@
     </row>
     <row r="2" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="76" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="76" t="s">
+      <c r="F2" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="76" t="s">
+      <c r="G2" s="76" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="76" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="76" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="76" t="s">
+      <c r="I2" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="H2" s="76" t="s">
+      <c r="J2" s="76" t="s">
         <v>62</v>
       </c>
-      <c r="I2" s="76" t="s">
+      <c r="K2" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="J2" s="76" t="s">
+      <c r="L2" s="76" t="s">
         <v>64</v>
-      </c>
-      <c r="K2" s="76" t="s">
-        <v>65</v>
-      </c>
-      <c r="L2" s="76" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3" spans="2:30" x14ac:dyDescent="0.25">
@@ -18233,34 +18233,34 @@
         <v>32</v>
       </c>
       <c r="C3" s="80" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="D3" s="80" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="80" t="s">
+      <c r="F3" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="80" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="80" t="s">
+      <c r="H3" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="80" t="s">
+      <c r="I3" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="I3" s="80" t="s">
+      <c r="J3" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="L3" s="80" t="s">
         <v>51</v>
-      </c>
-      <c r="J3" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="81" t="s">
-        <v>55</v>
-      </c>
-      <c r="L3" s="80" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.25">
@@ -20735,19 +20735,19 @@
   <sheetData>
     <row r="2" spans="2:15" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E2" s="75"/>
       <c r="F2" s="75"/>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H2" s="75"/>
       <c r="I2" s="75"/>
       <c r="J2" s="75"/>
       <c r="K2" s="75"/>
       <c r="L2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M2" s="75"/>
       <c r="N2" s="75"/>
@@ -34322,7 +34322,7 @@
         <v>0.93654855777826229</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J10" s="155"/>
       <c r="K10" s="156"/>
@@ -34540,7 +34540,7 @@
         <v>0.89904735637027922</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J18" s="155"/>
       <c r="K18" s="156"/>
@@ -34758,7 +34758,7 @@
         <v>0.92340466532845455</v>
       </c>
       <c r="I26" s="46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J26" s="155"/>
       <c r="K26" s="156"/>
@@ -35050,7 +35050,7 @@
         <v>8.761214173075393</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J37" s="12"/>
       <c r="M37" s="13"/>
@@ -35294,7 +35294,7 @@
         <v>13.939284927319285</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J45" s="12"/>
       <c r="M45" s="13"/>
@@ -35538,7 +35538,7 @@
         <v>10.576089498024002</v>
       </c>
       <c r="I53" s="46" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J53" s="12"/>
       <c r="M53" s="13"/>
@@ -35596,8 +35596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34CAD0DA-FC70-4D95-8264-ED6E1B5E9020}">
   <dimension ref="B2:AC63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35632,31 +35632,31 @@
         <v>32</v>
       </c>
       <c r="C4" s="80" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="80" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="80" t="s">
-        <v>47</v>
-      </c>
       <c r="E4" s="80" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F4" s="80" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G4" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="80" t="s">
+      <c r="I4" s="80" t="s">
+        <v>52</v>
+      </c>
+      <c r="J4" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="80" t="s">
         <v>51</v>
-      </c>
-      <c r="I4" s="80" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" s="81" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="80" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">

</xml_diff>